<commit_message>
optimized reading xlsx, clickable calendar
</commit_message>
<xml_diff>
--- a/test_out.xlsx
+++ b/test_out.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Period End</t>
   </si>
@@ -74,90 +74,6 @@
   </si>
   <si>
     <t>A20</t>
-  </si>
-  <si>
-    <t>0 9.8</t>
-  </si>
-  <si>
-    <t>0 0.8</t>
-  </si>
-  <si>
-    <t>4 3.5</t>
-  </si>
-  <si>
-    <t>9 3.1</t>
-  </si>
-  <si>
-    <t>9 8.6</t>
-  </si>
-  <si>
-    <t>11 6.3</t>
-  </si>
-  <si>
-    <t>11 15.2</t>
-  </si>
-  <si>
-    <t>16 15.8</t>
-  </si>
-  <si>
-    <t>17 14.8</t>
-  </si>
-  <si>
-    <t>19 11.2</t>
-  </si>
-  <si>
-    <t>20 0.7</t>
-  </si>
-  <si>
-    <t>3 14.3</t>
-  </si>
-  <si>
-    <t>3 13.8</t>
-  </si>
-  <si>
-    <t>4 15.1</t>
-  </si>
-  <si>
-    <t>9 3.9</t>
-  </si>
-  <si>
-    <t>13 1.2</t>
-  </si>
-  <si>
-    <t>18 0.7</t>
-  </si>
-  <si>
-    <t>2 4.2</t>
-  </si>
-  <si>
-    <t>4 14.1</t>
-  </si>
-  <si>
-    <t>4 6.1</t>
-  </si>
-  <si>
-    <t>5 1.4</t>
-  </si>
-  <si>
-    <t>9 10.9</t>
-  </si>
-  <si>
-    <t>10 10.8</t>
-  </si>
-  <si>
-    <t>11 2.2</t>
-  </si>
-  <si>
-    <t>13 3.3</t>
-  </si>
-  <si>
-    <t>14 2.9</t>
-  </si>
-  <si>
-    <t>17 9.3</t>
-  </si>
-  <si>
-    <t>1 4.4</t>
   </si>
 </sst>
 </file>
@@ -506,11 +422,11 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>42729</v>
+        <v>42739</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1">
-        <v>42733</v>
+        <v>42743</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -532,224 +448,140 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+    </row>
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+    </row>
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+    </row>
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+    </row>
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>14</v>
       </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+    </row>
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>14</v>
       </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+    </row>
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+    </row>
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>14</v>
       </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+    </row>
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+    </row>
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>15</v>
       </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+    </row>
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>16</v>
       </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+    </row>
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+    </row>
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>18</v>
       </c>
-      <c r="B29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+    </row>
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>19</v>
-      </c>
-      <c r="B30" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>